<commit_message>
✨ Agregar campo Sede de Registro al modelo de vehículo
- ✅ Nuevo enum SedeRegistro con 12 sedes (PUNO, AREQUIPA, JULIACA, etc.)
- ✅ Campo sedeRegistro agregado a todos los modelos de vehículo
- ✅ Validación de sede en carga masiva desde Excel
- ✅ Actualización de datos mock con sedes diversas
- ✅ Plantilla Excel actualizada con campo Sede de Registro
- ✅ Pruebas actualizadas y funcionando correctamente
- ✅ Documentación completa de relaciones del vehículo

Características implementadas:
- Sede por defecto: PUNO
- Validación en carga masiva de Excel
- 12 sedes disponibles para registro
- Integración completa en todo el sistema
- Resumen detallado de todas las relaciones del vehículo

El vehículo ahora tiene 12 tipos de relaciones principales:
1. Empresa (1:N), 2. Resolución (N:1), 3. Rutas (N:N)
4. TUC (1:1), 5. Documentos (1:N), 6. Historial (1:N)
7. Sede de Registro (N:1), 8. Datos Técnicos (1:1)
9-12. Enums: Categoría, Estado, Combustible, Sede
</commit_message>
<xml_diff>
--- a/backend/plantilla_vehiculos.xlsx
+++ b/backend/plantilla_vehiculos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,100 +461,105 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Sede de Registro</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Categoría</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Marca</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Modelo</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Año Fabricación</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Color</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Número Serie</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Motor</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Chasis</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Ejes</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Asientos</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Peso Neto (kg)</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Peso Bruto (kg)</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Largo (m)</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Ancho (m)</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Alto (m)</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Tipo Combustible</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Cilindrada</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Potencia (HP)</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Estado</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Observaciones</t>
         </is>
@@ -584,80 +589,85 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>PUNO</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>M3</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>MERCEDES BENZ</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>O500</t>
         </is>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>2020</v>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>BLANCO</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>MB123456</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>OM 457 LA</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>WDB9066131L123456</t>
         </is>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>2</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>50</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>8500</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>16000</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>12</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>2.55</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>3.2</v>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>DIESEL</t>
         </is>
       </c>
-      <c r="V2" t="n">
+      <c r="W2" t="n">
         <v>11967</v>
       </c>
-      <c r="W2" t="n">
+      <c r="X2" t="n">
         <v>354</v>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>ACTIVO</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>Vehículo de ejemplo</t>
         </is>
@@ -687,80 +697,85 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>AREQUIPA</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>N3</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>VOLVO</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>FH16</t>
         </is>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>2019</v>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>AZUL</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>VL789012</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>D16G750</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>VOLVOH16C123456</t>
         </is>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>3</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>2</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>12000</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>26000</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>16</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>2.6</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>3.8</v>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>DIESEL</t>
         </is>
       </c>
-      <c r="V3" t="n">
+      <c r="W3" t="n">
         <v>16000</v>
       </c>
-      <c r="W3" t="n">
+      <c r="X3" t="n">
         <v>750</v>
       </c>
-      <c r="X3" t="inlineStr">
+      <c r="Y3" t="inlineStr">
         <is>
           <t>ACTIVO</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="Z3" t="inlineStr">
         <is>
           <t>Camión de carga</t>
         </is>

</xml_diff>

<commit_message>
🔧 Reparación completa del frontend y sistema DataManager
✅ Correcciones Frontend:
- Corregida estructura DatosTecnicos en VehiculoService
- Aplicado optional chaining en dashboard component
- Corregidos métodos inexistentes (getVehiculoById → getVehiculo)
- Corregida integración con HistorialVehiculoService
- Eliminados imports innecesarios

🗄️ Sistema DataManager:
- Implementado DataManagerService completo
- Creado DataManagerClientService para frontend
- Dashboard de monitoreo con estadísticas en tiempo real
- Persistencia de datos en memoria durante desarrollo
- Integración completa backend-frontend

⚙️ Configuración:
- Entornos de desarrollo y producción configurados
- Flags de características habilitados
- URLs de API correctas

📁 Archivos de Prueba:
- test-frontend-completo.html
- test-dashboard-corregido.html
- test-datos-persistentes-completo.html
- test-errores-adicionales-corregidos.html

Estado: 0 errores TypeScript, compilación exitosa
</commit_message>
<xml_diff>
--- a/backend/plantilla_vehiculos.xlsx
+++ b/backend/plantilla_vehiculos.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
feat(mesa-partes): Complete Task 26 - Documentation and Deployment
- Task 26.1: Created comprehensive documentation
  * USER_GUIDE.md: Complete user manual in Spanish (500+ lines)
  * API_DOCUMENTATION.md: Full REST API reference (800+ lines)
  * INTEGRATION_GUIDE.md: Integration configuration guide (600+ lines)
  * DEPLOYMENT_GUIDE.md: Production deployment guide (700+ lines)

- Task 26.2: Prepared deployment infrastructure
  * Dockerfiles for backend and frontend (multi-stage builds)
  * Docker Compose files (main, production, monitoring)
  * Nginx configuration with SSL/TLS and security headers
  * CI/CD pipeline with GitHub Actions
  * Prometheus and Grafana monitoring stack
  * Environment configuration template
  * Alert rules and logging configuration

Total: 17 files created, 4,100+ lines of documentation and configuration
All requirements met, module ready for production deployment
</commit_message>
<xml_diff>
--- a/backend/plantilla_vehiculos.xlsx
+++ b/backend/plantilla_vehiculos.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>